<commit_message>
step-by-step document image locations modified
</commit_message>
<xml_diff>
--- a/examples/evpn_vxlan_erb_dc/dc1_data.xlsx
+++ b/examples/evpn_vxlan_erb_dc/dc1_data.xlsx
@@ -4918,8 +4918,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007500D8A1B389214CBED23636FE6E1CF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6ed09ef967e34e8533cad1c0a343467">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="901ad7fb-96f7-491c-a9c4-f5326a1d2890" xmlns:ns3="dbb7eb8b-91aa-4888-b096-f14d60c5e3a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8e466e2dd0b6e45a051c8a9ad7e7339" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007500D8A1B389214CBED23636FE6E1CF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65e57881ec998a134abc6600ab9e5dfb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="901ad7fb-96f7-491c-a9c4-f5326a1d2890" xmlns:ns3="dbb7eb8b-91aa-4888-b096-f14d60c5e3a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b2b410dd15ab9378e6c83352eb20d36" ns2:_="" ns3:_="">
     <xsd:import namespace="901ad7fb-96f7-491c-a9c4-f5326a1d2890"/>
     <xsd:import namespace="dbb7eb8b-91aa-4888-b096-f14d60c5e3a8"/>
     <xsd:element name="properties">
@@ -5127,10 +5127,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dbb7eb8b-91aa-4888-b096-f14d60c5e3a8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="901ad7fb-96f7-491c-a9c4-f5326a1d2890">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D1DFD51-5198-420E-9D17-73BC6FBB97AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FFF2ADA-2E1C-41E8-9C0A-4A657D8E2A3B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C19CA8C-102E-418B-9E2A-E6871FE95A33}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE705EC6-A5E0-4611-B865-FD1CB24F6CBE}"/>
 </file>
</xml_diff>